<commit_message>
alteração da escala do sistema solar
</commit_message>
<xml_diff>
--- a/calculo_raio.xlsx
+++ b/calculo_raio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MarcoSilva/Repositories/CG_1718/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B525F14-15B5-5A40-9AE6-64206AC6380D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AFD338-AD15-BE4F-AA07-61A666B9E84F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="440" windowWidth="25440" windowHeight="15020" xr2:uid="{4F61E350-1068-A744-AFF6-4FEF9E73B3CA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Raio total do sistema solar real -&gt;</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Raio do sol ao planeta virtual</t>
+  </si>
+  <si>
+    <t>Raio do sol</t>
   </si>
 </sst>
 </file>
@@ -72,9 +75,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,19 +393,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B810A94E-F6FF-7E48-89C3-102E0FCD2DAF}">
-  <dimension ref="D4:G5"/>
+  <dimension ref="D2:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="28.5" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2">
+        <v>676000</v>
+      </c>
+    </row>
     <row r="4" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>0</v>
@@ -410,7 +423,7 @@
         <v>5906123940</v>
       </c>
       <c r="F4">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
@@ -421,11 +434,11 @@
         <v>2</v>
       </c>
       <c r="E5" s="1">
-        <v>384400</v>
+        <v>57910000</v>
       </c>
       <c r="F5">
-        <f>((E5*F4)/E4) + 10</f>
-        <v>10.032542493512251</v>
+        <f>((E5*F4)/E4) + ((E2*F4)/E4)</f>
+        <v>9.9195344688279619</v>
       </c>
       <c r="G5" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
duas representações do sistema solar
</commit_message>
<xml_diff>
--- a/calculo_raio.xlsx
+++ b/calculo_raio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MarcoSilva/Repositories/CG_1718/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AFD338-AD15-BE4F-AA07-61A666B9E84F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE94E0B-B47E-134B-BCB7-25835C644956}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="440" windowWidth="25440" windowHeight="15020" xr2:uid="{4F61E350-1068-A744-AFF6-4FEF9E73B3CA}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="D2:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>